<commit_message>
PLS model verbeterd en loop over 5-13 factoren voor alle 4 main scripts.
</commit_message>
<xml_diff>
--- a/rmse_combined_pls.xlsx
+++ b/rmse_combined_pls.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3565112672059051</v>
+        <v>0.3565210559961738</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3566972550112256</v>
+        <v>0.3566961161843074</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3564649906567696</v>
+        <v>0.3564598914612215</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3564944424632374</v>
+        <v>0.3564955521839301</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.356923332799827</v>
+        <v>0.356911353007307</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3563006871689546</v>
+        <v>0.3563043392788862</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.3565909830251532</v>
+        <v>0.3565813169543481</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.3563632065945179</v>
+        <v>0.3563661354845151</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3568593224239394</v>
+        <v>0.3568557924782854</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3562983163622248</v>
+        <v>0.3562947154999627</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3564092078333679</v>
+        <v>0.3564068578878185</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.356632769089633</v>
+        <v>0.3566303133939332</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3568471403504346</v>
+        <v>0.3568403506571003</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.3566039514548474</v>
+        <v>0.3566016329033713</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.3569286524475823</v>
+        <v>0.3569297733533808</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.3570568363820158</v>
+        <v>0.3570607883658674</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.3567744076881071</v>
+        <v>0.3567852823364505</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.3566094789301918</v>
+        <v>0.3566127172934338</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.3567700496910422</v>
+        <v>0.3567682170408735</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.3569249572973142</v>
+        <v>0.356919880401531</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.3570228282135167</v>
+        <v>0.3570190182404508</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.3568158551269427</v>
+        <v>0.3568071262651077</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.3582248102017296</v>
+        <v>0.3582376118916283</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.3573736087053858</v>
+        <v>0.3573743441004111</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.3568661363043028</v>
+        <v>0.3568560843379328</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.357263316051864</v>
+        <v>0.3572523752525106</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.3576107211026032</v>
+        <v>0.357627856068959</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.3588243213844385</v>
+        <v>0.3588999483513917</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.3570243471060827</v>
+        <v>0.3570378007075127</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.3568570064331547</v>
+        <v>0.356845983277032</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.3571782305339732</v>
+        <v>0.3571771225275177</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.3571173998543755</v>
+        <v>0.3571210681559688</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.3567877109882631</v>
+        <v>0.3567908143499782</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.3571805489674206</v>
+        <v>0.3571807307345407</v>
       </c>
     </row>
     <row r="36">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.3571376162936832</v>
+        <v>0.3571378453116328</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.3570993807929978</v>
+        <v>0.3570989414306256</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.3570364685837119</v>
+        <v>0.3570352736651694</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.3569952189395629</v>
+        <v>0.3569937146210619</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.3571135291972295</v>
+        <v>0.3571059557308427</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.3570658387717511</v>
+        <v>0.3570661245029575</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.35701149944573</v>
+        <v>0.3570111600167287</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.3570594047493899</v>
+        <v>0.3570571032966088</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.3570341798557459</v>
+        <v>0.3570345441403476</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.3570214085346048</v>
+        <v>0.3570209707997928</v>
       </c>
     </row>
     <row r="46">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.3559739779329672</v>
+        <v>0.3559745276651449</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.3561431813881505</v>
+        <v>0.3561448494760212</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.3561382681168854</v>
+        <v>0.3561387742161629</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.3563005246580558</v>
+        <v>0.3563007401899932</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.3565791562957022</v>
+        <v>0.3565794883798692</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.3562299222262673</v>
+        <v>0.3562318282523075</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.3562299222262673</v>
+        <v>0.3562318282523075</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.3559764072639622</v>
+        <v>0.3559808806543016</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.3565132807010867</v>
+        <v>0.3565141947053384</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.3561037787780134</v>
+        <v>0.3561013750565168</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.3562991774608077</v>
+        <v>0.3562950821039401</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.356232701501513</v>
+        <v>0.3562358118194077</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.3562871380430545</v>
+        <v>0.3562932826266446</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.3563278787922268</v>
+        <v>0.3563312244421296</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.3565868239624884</v>
+        <v>0.3565888569493826</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.3568572790080689</v>
+        <v>0.3568574979387144</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.356072264650322</v>
+        <v>0.3560694540125161</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.3565743335386718</v>
+        <v>0.3565781698818984</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.3562081045910433</v>
+        <v>0.3562174285919251</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.3566986486539099</v>
+        <v>0.3567013519267569</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.3563962811568898</v>
+        <v>0.3563922566159613</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.3564687706181474</v>
+        <v>0.3564666501649183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>